<commit_message>
Good solid version before streamlit
</commit_message>
<xml_diff>
--- a/outputs/template.xlsx
+++ b/outputs/template.xlsx
@@ -43,72 +43,84 @@
     <t>Supported</t>
   </si>
   <si>
+    <t>Skip Logic</t>
+  </si>
+  <si>
+    <t>Answer Q6 if Q4 is Ontario</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>183, 590, 615, 653</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>Mandatory Logic</t>
   </si>
   <si>
     <t>Block Q49 if Q48r97 selected</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>250</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Skip Logic</t>
-  </si>
-  <si>
-    <t>Answer  Q6 if Q4 is Ontario</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>183, 590, 615, 653</t>
-  </si>
-  <si>
     <t>Exclusive</t>
   </si>
   <si>
     <t>Selecting one answer prevents the selection of any other options.</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>21, 99, 100, 127, 147, 163, 190, 209, 316, 319, 351, 400, 410, 452, 516, 517, 585, 591, 606, 610, 622, 627, 631, 644, 687, 689, 705, 744, 770, 798, 802, 814, 827, 831, 840, 845, 846, 858, 876, 883, 986</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>757, 909</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44, 57, 72, 81, 84, 93, 99, 152, 155, 290, 351, 393, 396, 397, 400, 401, 431, 432, 452, 467, 489, 524, 565, 631, 646, 656, 670, 689, 691, 701, 727, 744, 766, 770, 807, 810, 824, 876, 901, 908, 940, 946, 996</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
     <t>132, 810, 946</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>44, 57, 72, 81, 84, 93, 99, 152, 155, 290, 351, 393, 396, 397, 400, 401, 431, 432, 452, 467, 489, 524, 565, 631, 646, 656, 670, 689, 691, 701, 727, 744, 766, 770, 807, 810, 824, 876, 901, 908, 940, 946, 996</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>757, 909</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>21, 99, 100, 127, 147, 163, 190, 209, 316, 319, 351, 400, 410, 452, 516, 517, 585, 591, 606, 610, 622, 627, 631, 644, 687, 689, 705, 744, 770, 798, 802, 814, 827, 831, 840, 845, 846, 858, 876, 883, 986</t>
-  </si>
-  <si>
     <t>Recodes/Hidden Variables</t>
   </si>
   <si>
+    <t>Recoding from birthdate to age - many values for the same recode issue</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>467</t>
+  </si>
+  <si>
+    <t>0, 8, 9, 11, 13, 16, 17, 19, 21, 22, 23, 30, 31, 35, 37, 39, 40, 41, 43, 44, 45, 46, 49, 55, 56, 57, 58, 59, 60, 63, 64, 66, 72, 74, 75, 80, 81, 82, 83, 84, 85, 88, 89, 91, 93, 94, 97, 99, 102, 108, 109, 110, 112, 115, 119, 123, 127, 128, 129, 130, 131, 132, 136, 147, 150, 151, 152, 153, 154, 155, 156, 157, 160, 161, 163, 165, 169, 172, 174, 176, 177, 178, 180, 183, 184, 189, 190, 191, 195, 197, 202, 204, 205, 209, 212, 215, 217, 218, 220, 221, 225, 228, 230, 231, 233, 234, 235, 238, 240, 241, 242, 245, 249, 250, 255, 259, 262, 263, 266, 268, 271, 272, 275, 277, 278, 280, 284, 285, 288, 290, 291, 295, 298, 299, 302, 304, 310, 313, 314, 316, 318, 319, 320, 324, 325, 326, 327, 329, 330, 333, 336, 339, 340, 342, 343, 345, 346, 347, 350, 351, 353, 355, 357, 358, 360, 364, 367, 369, 372, 373, 376, 379, 384, 386, 388, 392, 393, 394, 395, 396, 397, 398, 400, 401, 404, 406, 409, 410, 413, 414, 416, 417, 421, 424, 425, 426, 427, 428, 429, 431, 432, 433, 437, 438, 440, 442, 443, 444, 446, 450, 452, 454, 455, 460, 466, 467, 469, 473, 480, 482, 484, 486, 487, 488, 489, 490, 492, 494, 495, 496, 497, 498, 499, 501, 502, 503, 505, 509, 513, 514, 516, 517, 518, 521, 522, 523, 524, 525, 526, 527, 532, 534, 537, 538, 539, 541, 544, 545, 546, 547, 549, 550, 553, 555, 556, 558, 560, 564, 565, 572, 575, 578, 579, 584, 585, 589, 590, 591, 592, 595, 596, 599, 602, 604, 606, 608, 610, 614, 615, 619, 624, 626, 627, 628, 629, 630, 631, 633, 634, 635, 636, 644, 646, 647, 652, 653, 655, 656, 658, 660, 667, 669, 670, 673, 675, 678, 680, 681, 683, 685, 687, 688, 689, 691, 693, 696, 700, 701, 702, 705, 707, 708, 709, 710, 712, 714, 721, 725, 727, 728, 730, 733, 734, 735, 737, 741, 743, 744, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 759, 765, 766, 769, 770, 773, 775, 779, 780, 782, 783, 784, 785, 786, 787, 790, 794, 797, 798, 801, 802, 803, 807, 808, 809, 810, 812, 814, 818, 819, 823, 824, 826, 827, 828, 831, 834, 835, 836, 840, 842, 843, 846, 848, 852, 855, 858, 865, 867, 869, 871, 874, 876, 881, 882, 883, 884, 885, 887, 889, 891, 894, 896, 898, 899, 901, 902, 905, 908, 909, 914, 916, 923, 927, 928, 931, 932, 935, 936, 940, 946, 949, 950, 952, 954, 956, 959, 961, 963, 964, 965, 966, 967, 972, 974, 975, 977, 978, 980, 982, 986, 988, 990, 992, 995, 996, 997, 998, 999</t>
+  </si>
+  <si>
     <t>Recoding Age to age groups - many values for the same code issue (value 9999.0 causing the issue)</t>
   </si>
   <si>
@@ -151,18 +163,6 @@
     <t>30, 37, 40, 95, 127, 132, 136, 172, 174, 177, 209, 233, 274, 330, 343, 350, 373, 400, 414, 484, 522, 534, 545, 683, 687, 956, 986</t>
   </si>
   <si>
-    <t>Recoding from birthdate to age - many values for the same recode issue</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>467</t>
-  </si>
-  <si>
-    <t>0, 8, 9, 11, 13, 16, 17, 19, 21, 22, 23, 30, 31, 35, 37, 39, 40, 41, 43, 44, 45, 46, 49, 55, 56, 57, 58, 59, 60, 63, 64, 66, 72, 74, 75, 80, 81, 82, 83, 84, 85, 88, 89, 91, 93, 94, 97, 99, 102, 108, 109, 110, 112, 115, 119, 123, 127, 128, 129, 130, 131, 132, 136, 147, 150, 151, 152, 153, 154, 155, 156, 157, 160, 161, 163, 165, 169, 172, 174, 176, 177, 178, 180, 183, 184, 189, 190, 191, 195, 197, 202, 204, 205, 209, 212, 215, 217, 218, 220, 221, 225, 228, 230, 231, 233, 234, 235, 238, 240, 241, 242, 245, 249, 250, 255, 259, 262, 263, 266, 268, 271, 272, 275, 277, 278, 280, 284, 285, 288, 290, 291, 295, 298, 299, 302, 304, 310, 313, 314, 316, 318, 319, 320, 324, 325, 326, 327, 329, 330, 333, 336, 339, 340, 342, 343, 345, 346, 347, 350, 351, 353, 355, 357, 358, 360, 364, 367, 369, 372, 373, 376, 379, 384, 386, 388, 392, 393, 394, 395, 396, 397, 398, 400, 401, 404, 406, 409, 410, 413, 414, 416, 417, 421, 424, 425, 426, 427, 428, 429, 431, 432, 433, 437, 438, 440, 442, 443, 444, 446, 450, 452, 454, 455, 460, 466, 467, 469, 473, 480, 482, 484, 486, 487, 488, 489, 490, 492, 494, 495, 496, 497, 498, 499, 501, 502, 503, 505, 509, 513, 514, 516, 517, 518, 521, 522, 523, 524, 525, 526, 527, 532, 534, 537, 538, 539, 541, 544, 545, 546, 547, 549, 550, 553, 555, 556, 558, 560, 564, 565, 572, 575, 578, 579, 584, 585, 589, 590, 591, 592, 595, 596, 599, 602, 604, 606, 608, 610, 614, 615, 619, 624, 626, 627, 628, 629, 630, 631, 633, 634, 635, 636, 644, 646, 647, 652, 653, 655, 656, 658, 660, 667, 669, 670, 673, 675, 678, 680, 681, 683, 685, 687, 688, 689, 691, 693, 696, 700, 701, 702, 705, 707, 708, 709, 710, 712, 714, 721, 725, 727, 728, 730, 733, 734, 735, 737, 741, 743, 744, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 759, 765, 766, 769, 770, 773, 775, 779, 780, 782, 783, 784, 785, 786, 787, 790, 794, 797, 798, 801, 802, 803, 807, 808, 809, 810, 812, 814, 818, 819, 823, 824, 826, 827, 828, 831, 834, 835, 836, 840, 842, 843, 846, 848, 852, 855, 858, 865, 867, 869, 871, 874, 876, 881, 882, 883, 884, 885, 887, 889, 891, 894, 896, 898, 899, 901, 902, 905, 908, 909, 914, 916, 923, 927, 928, 931, 932, 935, 936, 940, 946, 949, 950, 952, 954, 956, 959, 961, 963, 964, 965, 966, 967, 972, 974, 975, 977, 978, 980, 982, 986, 988, 990, 992, 995, 996, 997, 998, 999</t>
-  </si>
-  <si>
     <t>Selection Limit Control</t>
   </si>
   <si>
@@ -178,6 +178,15 @@
     <t>2, 6, 10, 18, 27, 40, 44, 52, 54, 62, 65, 67, 77, 79, 84, 86, 89, 93, 94, 96, 103, 104, 106, 110, 113, 116, 118, 123, 125, 135, 143, 145, 150, 159, 164, 170, 193, 207, 213, 219, 223, 226, 239, 243, 265, 269, 283, 285, 286, 288, 292, 293, 301, 305, 306, 311, 313, 322, 326, 328, 332, 337, 346, 356, 358, 361, 362, 363, 364, 370, 374, 375, 390, 396, 397, 399, 402, 405, 418, 420, 423, 431, 432, 451, 453, 456, 458, 461, 464, 470, 474, 483, 489, 493, 503, 504, 510, 511, 514, 536, 540, 548, 552, 562, 565, 566, 567, 573, 581, 582, 583, 594, 597, 605, 609, 613, 616, 618, 621, 623, 633, 637, 641, 643, 652, 656, 663, 664, 665, 670, 677, 686, 694, 695, 699, 701, 702, 703, 706, 711, 713, 716, 717, 720, 722, 723, 724, 734, 740, 741, 742, 747, 758, 760, 761, 762, 764, 774, 778, 782, 797, 799, 817, 829, 833, 839, 847, 851, 854, 861, 870, 872, 878, 889, 890, 892, 897, 900, 901, 908, 911, 912, 919, 924, 945, 947, 948, 962, 965, 969, 970, 983, 985, 989, 991, 996</t>
   </si>
   <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>13, 18, 19, 21, 73, 84, 93, 99, 155, 159, 174, 215, 329, 337, 353, 394, 397, 413, 424, 442, 499, 502, 539, 541, 546, 556, 606, 680, 689, 691, 748, 751, 757, 766, 801, 802, 812, 814, 824, 848, 884, 885, 898, 964</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
     <t>6</t>
   </si>
   <si>
@@ -185,15 +194,6 @@
   </si>
   <si>
     <t>50, 63, 72, 80, 91, 129, 131, 165, 184, 209, 228, 235, 266, 274, 301, 319, 353, 360, 391, 398, 400, 406, 429, 440, 442, 454, 495, 498, 517, 524, 525, 527, 538, 585, 596, 630, 644, 693, 730, 749, 769, 780, 785, 827, 858, 865, 871, 894, 899, 914, 978, 982, 986</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>13, 18, 19, 21, 73, 84, 93, 99, 155, 159, 174, 215, 329, 337, 353, 394, 397, 413, 424, 442, 499, 502, 539, 541, 546, 556, 606, 680, 689, 691, 748, 751, 757, 766, 801, 802, 812, 814, 824, 848, 884, 885, 898, 964</t>
   </si>
   <si>
     <t>Number of rows affected: 636</t>
@@ -664,33 +664,33 @@
         <v>11</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="20" customHeight="1">
       <c r="B10" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="45" customHeight="1">
@@ -701,16 +701,16 @@
         <v>19</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="45" customHeight="1">
@@ -721,16 +721,16 @@
         <v>19</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="45" customHeight="1">
@@ -741,7 +741,7 @@
         <v>19</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>26</v>
@@ -750,7 +750,7 @@
         <v>27</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="45" customHeight="1">
@@ -761,7 +761,7 @@
         <v>19</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>28</v>
@@ -770,10 +770,10 @@
         <v>29</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="60" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="45" customHeight="1">
       <c r="B15" s="4" t="s">
         <v>30</v>
       </c>
@@ -790,10 +790,10 @@
         <v>34</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="45" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="60" customHeight="1">
       <c r="B16" s="4" t="s">
         <v>30</v>
       </c>
@@ -810,10 +810,10 @@
         <v>38</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="20" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="45" customHeight="1">
       <c r="B17" s="4" t="s">
         <v>30</v>
       </c>
@@ -821,47 +821,47 @@
         <v>39</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="60" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="20" customHeight="1">
       <c r="B18" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="45" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="60" customHeight="1">
       <c r="B19" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>47</v>
@@ -870,7 +870,7 @@
         <v>48</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="45" customHeight="1">
@@ -890,34 +890,34 @@
         <v>53</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="20" customHeight="1">
       <c r="B21" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="G21" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="20" customHeight="1">
       <c r="B22" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>58</v>
@@ -926,7 +926,7 @@
         <v>59</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="2:7">

</xml_diff>